<commit_message>
Add test queries to questions excel
</commit_message>
<xml_diff>
--- a/Questions.xlsx
+++ b/Questions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neo/Desktop/text2sql/text2sql_prod/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neo/Desktop/DataWorksAI/text2sql_prod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15EFA57-DBEA-0A48-A252-BEE680780C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE90B7D7-8F81-5E43-A994-3EAF117C72D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16040" xr2:uid="{AEEAE0F9-1A2B-0C42-B685-E0A53EC39443}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">Human Language </t>
   </si>
@@ -50,6 +50,14 @@
     <t>SELECT COUNT(*) 
 FROM hd2022 
 WHERE city = 'Boston';</t>
+  </si>
+  <si>
+    <t>What is the address of the University of California, Berkeley?</t>
+  </si>
+  <si>
+    <t>SELECT pcaddr
+FROM ic2022campuses
+WHERE pcinstnm = 'University of California, Berkeley';</t>
   </si>
 </sst>
 </file>
@@ -424,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418D210D-A9F4-C34A-9D63-AC1F08C1D997}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -452,6 +460,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Push one more time to see results
</commit_message>
<xml_diff>
--- a/Questions.xlsx
+++ b/Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neo/Desktop/DataWorksAI/text2sql_prod/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE90B7D7-8F81-5E43-A994-3EAF117C72D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EFC8D4-12D4-D94B-956F-8520BB6FE287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16040" xr2:uid="{AEEAE0F9-1A2B-0C42-B685-E0A53EC39443}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t xml:space="preserve">Human Language </t>
   </si>
@@ -58,13 +58,102 @@
     <t>SELECT pcaddr
 FROM ic2022campuses
 WHERE pcinstnm = 'University of California, Berkeley';</t>
+  </si>
+  <si>
+    <t>What is the total number of institutions listed in the dataset?</t>
+  </si>
+  <si>
+    <t>Can you find the street address for Stanford University?</t>
+  </si>
+  <si>
+    <t>List all institutions in california</t>
+  </si>
+  <si>
+    <t>Which states have the highest number of institutions?</t>
+  </si>
+  <si>
+    <t>Are there any institutions in Alaska?</t>
+  </si>
+  <si>
+    <t>Identify institutions that do not participate in Title IV but have a deferment agreement.</t>
+  </si>
+  <si>
+    <t>How many institutions are currently not active?</t>
+  </si>
+  <si>
+    <t>What is the identification number for Harvard University?</t>
+  </si>
+  <si>
+    <t>Top 10 research universities.</t>
+  </si>
+  <si>
+    <t>Top 5 research universities in massachusetts</t>
+  </si>
+  <si>
+    <t>How many institutions are located in rural versus urban areas?</t>
+  </si>
+  <si>
+    <t>SELECT pcaddr
+FROM ic2022campusesWHERE pcinstnm = 'University of California, Berkeley';</t>
+  </si>
+  <si>
+    <t>SELECT ADDR
+FROM hd2022
+WHERE INSTNM = 'Stanford University';</t>
+  </si>
+  <si>
+    <t>SELECT instnm
+FROM hd2022
+WHERE stabbr = 'CA';</t>
+  </si>
+  <si>
+    <t>SELECT stabbr, COUNT(unitid) 
+FROM hd2022
+GROUP BY stabbr
+ORDER BY COUNT(unitid) DESC;</t>
+  </si>
+  <si>
+    <t>SELECT COUNT(*) 
+FROM hd2022 
+WHERE stabbr = 'AK';</t>
+  </si>
+  <si>
+    <t>SELECT pcinstnm
+FROM ic2022campuses
+WHERE pcopeflag = 0;</t>
+  </si>
+  <si>
+    <t>SELECT COUNT(*)
+FROM ic2022campuses
+WHERE pcact = "1";</t>
+  </si>
+  <si>
+    <t>SELECT unitid
+FROM hd2022
+WHERE instnm = 'Harvard University';</t>
+  </si>
+  <si>
+    <t>SELECT hd.instnm
+FROM hd2022 hd
+WHERE hd.c15basic = 15
+ORDER BY hd.c18basic DESC
+LIMIT 10;</t>
+  </si>
+  <si>
+    <t>SELECT locale, COUNT(*) 
+FROM hd2022 
+GROUP BY locale;</t>
+  </si>
+  <si>
+    <t>SELECT COUNT(unitid) AS total_institutions
+FROM hd2022;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -72,16 +161,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F3F3"/>
+        <bgColor rgb="FFF3F3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -89,14 +196,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -432,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418D210D-A9F4-C34A-9D63-AC1F08C1D997}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -468,6 +596,102 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="85" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="68" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>